<commit_message>
Update spreadsheet of UART message bytes
</commit_message>
<xml_diff>
--- a/GardenPiUARTByteAllotment.xlsx
+++ b/GardenPiUARTByteAllotment.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="198" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="395" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>GardenPi UART Byte Allotment</t>
   </si>
@@ -26,33 +26,60 @@
     <t>0x00</t>
   </si>
   <si>
+    <t>Null Byte</t>
+  </si>
+  <si>
     <t>0x01</t>
   </si>
   <si>
+    <t>RasPi initialize request to AVR</t>
+  </si>
+  <si>
     <t>0x02</t>
   </si>
   <si>
+    <t>AVR initialize handshake to RasPi</t>
+  </si>
+  <si>
     <t>0x03</t>
   </si>
   <si>
     <t>0x04</t>
   </si>
   <si>
+    <t>RasPi request AVR</t>
+  </si>
+  <si>
     <t>0x05</t>
   </si>
   <si>
+    <t>AVR request RasPi</t>
+  </si>
+  <si>
     <t>0x06</t>
   </si>
   <si>
+    <t>RasPi ready to receive</t>
+  </si>
+  <si>
     <t>0x07</t>
   </si>
   <si>
+    <t>AVR ready to receive</t>
+  </si>
+  <si>
     <t>0x08</t>
   </si>
   <si>
+    <t>RasPi message receipt confirmation</t>
+  </si>
+  <si>
     <t>0x09</t>
   </si>
   <si>
+    <t>AVR message receipt confirmation</t>
+  </si>
+  <si>
     <t>0x0A</t>
   </si>
   <si>
@@ -173,19 +200,34 @@
     <t>Select option 16</t>
   </si>
   <si>
-    <t>Moisture Sensor Messages</t>
+    <t>Sensor Request Messages</t>
+  </si>
+  <si>
+    <t>0x20</t>
+  </si>
+  <si>
+    <t>Water Tank Level</t>
   </si>
   <si>
     <t>0x30</t>
   </si>
   <si>
+    <t>Soil Moisture</t>
+  </si>
+  <si>
     <t>Error Messages</t>
   </si>
   <si>
     <t>0xF0</t>
   </si>
   <si>
+    <t>UART communication error</t>
+  </si>
+  <si>
     <t>0xF1</t>
+  </si>
+  <si>
+    <t>Ultrasonic range sensor timeout error</t>
   </si>
   <si>
     <t>0xF2</t>
@@ -242,6 +284,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -263,12 +306,14 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -347,10 +392,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -374,216 +419,243 @@
       <c r="A4" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -591,97 +663,114 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="s">
-        <v>54</v>
+        <v>62</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>55</v>
+      <c r="A43" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>56</v>
+        <v>67</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>57</v>
+        <v>69</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>70</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>